<commit_message>
Nf Ref for Ng=0
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/calibration20161012.xlsx
+++ b/myESC-Particle-DEV/saves/calibration20161012.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9972" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CalArduino" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>Test Data</t>
   </si>
   <si>
-    <t>cover observed Nf,% and Throttle, deg ranges</t>
-  </si>
-  <si>
     <t>what works</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>cal thtl</t>
+  </si>
+  <si>
+    <t>Nf for 0% Ng</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -723,9 +723,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -741,7 +738,6 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -790,6 +786,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,11 +1011,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80788976"/>
-        <c:axId val="80791328"/>
+        <c:axId val="193840256"/>
+        <c:axId val="193837904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80788976"/>
+        <c:axId val="193840256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,12 +1128,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80791328"/>
+        <c:crossAx val="193837904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80791328"/>
+        <c:axId val="193837904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1240,7 +1246,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80788976"/>
+        <c:crossAx val="193840256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1521,11 +1527,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="80784272"/>
-        <c:axId val="80784664"/>
+        <c:axId val="193835552"/>
+        <c:axId val="193837120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="80784272"/>
+        <c:axId val="193835552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1582,12 +1588,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80784664"/>
+        <c:crossAx val="193837120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80784664"/>
+        <c:axId val="193837120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1644,7 +1650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80784272"/>
+        <c:crossAx val="193835552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1819,7 +1825,43 @@
             <c:forward val="5.5"/>
             <c:backward val="20"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.5478196039448559E-2"/>
+                  <c:y val="0.1523936574043947"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -1891,14 +1933,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="219731744"/>
-        <c:axId val="225401784"/>
+        <c:axId val="193837512"/>
+        <c:axId val="193838296"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="219731744"/>
+        <c:axId val="193837512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="50"/>
+          <c:max val="180"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1937,8 +1980,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>ln(Throttle)</a:t>
+                  <a:t>Throttle,</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> deg</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2009,12 +2057,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225401784"/>
+        <c:crossAx val="193838296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225401784"/>
+        <c:axId val="193838296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2127,7 +2175,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="219731744"/>
+        <c:crossAx val="193837512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2191,6 +2239,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Power </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Follows Square Law</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -2299,27 +2367,46 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="225398648"/>
-        <c:axId val="225401000"/>
+        <c:axId val="193839864"/>
+        <c:axId val="193841432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="225398648"/>
+        <c:axId val="193839864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Ng, %</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225401000"/>
+        <c:crossAx val="193841432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225401000"/>
+        <c:axId val="193841432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2330,7 +2417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225398648"/>
+        <c:crossAx val="193839864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2461,11 +2548,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="225401392"/>
-        <c:axId val="225397472"/>
+        <c:axId val="195149472"/>
+        <c:axId val="195151040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="225401392"/>
+        <c:axId val="195149472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2475,12 +2562,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225397472"/>
+        <c:crossAx val="195151040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225397472"/>
+        <c:axId val="195151040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2491,7 +2578,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="225401392"/>
+        <c:crossAx val="195149472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2732,11 +2819,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="225399040"/>
-        <c:axId val="225402568"/>
+        <c:axId val="195151432"/>
+        <c:axId val="195154568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="225399040"/>
+        <c:axId val="195151432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2849,12 +2936,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225402568"/>
+        <c:crossAx val="195154568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="225402568"/>
+        <c:axId val="195154568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2968,7 +3055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="225399040"/>
+        <c:crossAx val="195151432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5245,16 +5332,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>30480</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5275,16 +5362,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5305,16 +5392,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>422910</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>53346</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>87630</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>22866</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>102870</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>45726</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>186690</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>60966</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5335,16 +5422,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>280035</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>62871</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>302895</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>177171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>80010</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>131451</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>64770</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>40011</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5365,16 +5452,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>76206</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>169545</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>167646</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161931</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>70491</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5400,16 +5487,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5722,9 +5809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X2" sqref="X2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5765,28 +5852,28 @@
       <c r="A1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="78" t="s">
+      <c r="B1" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="78" t="s">
+      <c r="G1" s="76" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="78" t="s">
+      <c r="H1" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="I1" s="77" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="4" t="s">
@@ -5839,50 +5926,50 @@
         <v>Charger Pwr, W</v>
       </c>
       <c r="Z1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="B2" s="80">
+      <c r="B2" s="78">
         <v>1.4338333333333333</v>
       </c>
-      <c r="C2" s="76">
+      <c r="C2" s="74">
         <v>78.089999999999989</v>
       </c>
-      <c r="D2" s="76">
+      <c r="D2" s="74">
         <v>0.5</v>
       </c>
-      <c r="E2" s="76">
+      <c r="E2" s="74">
         <v>12</v>
       </c>
-      <c r="F2" s="76">
+      <c r="F2" s="74">
         <v>0.97</v>
       </c>
-      <c r="G2" s="76">
+      <c r="G2" s="74">
         <v>3840</v>
       </c>
-      <c r="H2" s="76">
+      <c r="H2" s="74">
         <v>9150</v>
       </c>
-      <c r="I2" s="81">
+      <c r="I2" s="79">
         <v>3.2</v>
       </c>
       <c r="J2" s="2">
@@ -5963,28 +6050,28 @@
       </c>
     </row>
     <row r="3" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="80">
+      <c r="B3" s="78">
         <v>1.4649999999999999</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="74">
         <v>83.699999999999974</v>
       </c>
-      <c r="D3" s="76">
+      <c r="D3" s="74">
         <v>0.74199999999999999</v>
       </c>
-      <c r="E3" s="76">
+      <c r="E3" s="74">
         <v>12</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="74">
         <v>1.51</v>
       </c>
-      <c r="G3" s="76">
+      <c r="G3" s="74">
         <v>3180</v>
       </c>
-      <c r="H3" s="76">
+      <c r="H3" s="74">
         <v>6060</v>
       </c>
-      <c r="I3" s="81">
+      <c r="I3" s="79">
         <v>4.5999999999999996</v>
       </c>
       <c r="J3" s="2">
@@ -6080,28 +6167,28 @@
       </c>
     </row>
     <row r="4" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="80">
+      <c r="B4" s="78">
         <v>1.568888888888889</v>
       </c>
-      <c r="C4" s="76">
+      <c r="C4" s="74">
         <v>102.40000000000002</v>
       </c>
-      <c r="D4" s="76">
+      <c r="D4" s="74">
         <v>1.17</v>
       </c>
-      <c r="E4" s="76">
+      <c r="E4" s="74">
         <v>12</v>
       </c>
-      <c r="F4" s="76">
+      <c r="F4" s="74">
         <v>3</v>
       </c>
-      <c r="G4" s="76">
+      <c r="G4" s="74">
         <v>2450</v>
       </c>
-      <c r="H4" s="76">
+      <c r="H4" s="74">
         <v>3840</v>
       </c>
-      <c r="I4" s="81">
+      <c r="I4" s="79">
         <v>7.4</v>
       </c>
       <c r="J4" s="2">
@@ -6197,28 +6284,28 @@
       </c>
     </row>
     <row r="5" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="80">
+      <c r="B5" s="78">
         <v>1.6727777777777779</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="74">
         <v>121.10000000000002</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="74">
         <v>1.52</v>
       </c>
-      <c r="E5" s="76">
+      <c r="E5" s="74">
         <v>12</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="74">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G5" s="76">
+      <c r="G5" s="74">
         <v>2000</v>
       </c>
-      <c r="H5" s="76">
+      <c r="H5" s="74">
         <v>2980</v>
       </c>
-      <c r="I5" s="81">
+      <c r="I5" s="79">
         <v>9.4</v>
       </c>
       <c r="J5" s="2">
@@ -6314,28 +6401,28 @@
       </c>
     </row>
     <row r="6" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="80">
+      <c r="B6" s="78">
         <v>1.7143333333333333</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="74">
         <v>128.57999999999998</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="74">
         <v>1.7</v>
       </c>
-      <c r="E6" s="76">
+      <c r="E6" s="74">
         <v>12</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="74">
         <v>5.4</v>
       </c>
-      <c r="G6" s="76">
+      <c r="G6" s="74">
         <v>1930</v>
       </c>
-      <c r="H6" s="76">
+      <c r="H6" s="74">
         <v>2760</v>
       </c>
-      <c r="I6" s="81">
+      <c r="I6" s="79">
         <v>10.4</v>
       </c>
       <c r="J6" s="2">
@@ -6431,28 +6518,28 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="80">
+      <c r="B7" s="78">
         <v>1.8545833333333333</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="74">
         <v>153.82499999999999</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="74">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="74">
         <v>12</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="74">
         <v>8.6999999999999993</v>
       </c>
-      <c r="G7" s="76">
+      <c r="G7" s="74">
         <v>1610</v>
       </c>
-      <c r="H7" s="76">
+      <c r="H7" s="74">
         <v>2180</v>
       </c>
-      <c r="I7" s="81">
+      <c r="I7" s="79">
         <v>13</v>
       </c>
       <c r="J7" s="2">
@@ -6533,28 +6620,28 @@
       </c>
     </row>
     <row r="8" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="82">
+      <c r="B8" s="80">
         <v>1.9470444444444444</v>
       </c>
-      <c r="C8" s="83">
+      <c r="C8" s="81">
         <v>170.46799999999999</v>
       </c>
-      <c r="D8" s="83">
+      <c r="D8" s="81">
         <v>2.71</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="81">
         <v>12</v>
       </c>
-      <c r="F8" s="83">
+      <c r="F8" s="81">
         <v>13</v>
       </c>
-      <c r="G8" s="83">
+      <c r="G8" s="81">
         <v>1408</v>
       </c>
-      <c r="H8" s="83">
+      <c r="H8" s="81">
         <v>1880</v>
       </c>
-      <c r="I8" s="84">
+      <c r="I8" s="82">
         <v>15</v>
       </c>
       <c r="J8" s="2">
@@ -6636,7 +6723,7 @@
     </row>
     <row r="9" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AC9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD9">
         <f>AVERAGE(AD3:AD6)</f>
@@ -6709,9 +6796,14 @@
       </c>
     </row>
     <row r="12" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -6752,9 +6844,12 @@
       <c r="AL12" s="29"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -6796,9 +6891,12 @@
       <c r="AL13" s="31"/>
     </row>
     <row r="14" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -6813,14 +6911,6 @@
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
       <c r="Y14" s="3"/>
       <c r="AA14" s="21" t="s">
         <v>5</v>
@@ -6861,12 +6951,6 @@
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
       <c r="Y15" s="3"/>
     </row>
     <row r="16" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -6887,12 +6971,6 @@
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
       <c r="Y16" s="3"/>
       <c r="AA16" t="s">
         <v>53</v>
@@ -7060,11 +7138,12 @@
       <c r="AJ21" s="60">
         <v>0</v>
       </c>
-      <c r="AK21" s="61">
-        <v>-5</v>
+      <c r="AK21" s="90">
+        <f>AE23/AB17*100</f>
+        <v>-17.719588605194325</v>
       </c>
       <c r="AL21" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="2:41" x14ac:dyDescent="0.3">
@@ -7159,13 +7238,13 @@
       </c>
       <c r="AG23" s="19"/>
       <c r="AH23" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI23" s="30"/>
       <c r="AJ23" s="62"/>
-      <c r="AK23" s="63">
+      <c r="AK23" s="90">
         <f>(AK22-AK21)/(AH22-AH21)</f>
-        <v>15</v>
+        <v>17.543917721038866</v>
       </c>
     </row>
     <row r="24" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7204,9 +7283,9 @@
       <c r="AH24" s="30"/>
       <c r="AI24" s="30"/>
       <c r="AJ24" s="62"/>
-      <c r="AK24" s="63">
+      <c r="AK24" s="90">
         <f>AK22-AK23*(AH22-AH21)</f>
-        <v>-5</v>
+        <v>-17.719588605194332</v>
       </c>
     </row>
     <row r="25" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -7243,13 +7322,13 @@
     </row>
     <row r="26" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -7279,14 +7358,14 @@
       <c r="AC26" s="5"/>
     </row>
     <row r="27" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B27" s="76">
+      <c r="B27" s="74">
         <v>87</v>
       </c>
       <c r="C27" s="6">
         <f>B27/180*(2.4-0.53)+0.53</f>
         <v>1.4338333333333333</v>
       </c>
-      <c r="D27" s="91">
+      <c r="D27" s="89">
         <f>(C27-1)*180</f>
         <v>78.089999999999989</v>
       </c>
@@ -7311,25 +7390,25 @@
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
-      <c r="AA27" s="64" t="s">
+      <c r="AA27" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="AB27" s="65">
+      <c r="AB27" s="64">
         <f>AH22</f>
         <v>5</v>
       </c>
-      <c r="AC27" s="66"/>
+      <c r="AC27" s="65"/>
       <c r="AD27" s="29"/>
     </row>
     <row r="28" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B28" s="76">
+      <c r="B28" s="74">
         <v>90</v>
       </c>
       <c r="C28" s="6">
         <f t="shared" ref="C28:C33" si="19">B28/180*(2.4-0.53)+0.53</f>
         <v>1.4649999999999999</v>
       </c>
-      <c r="D28" s="91">
+      <c r="D28" s="89">
         <f t="shared" ref="D28:D33" si="20">(C28-1)*180</f>
         <v>83.699999999999974</v>
       </c>
@@ -7354,10 +7433,10 @@
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10"/>
-      <c r="AA28" s="67" t="s">
+      <c r="AA28" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="AB28" s="68">
+      <c r="AB28" s="67">
         <f>AH21</f>
         <v>0</v>
       </c>
@@ -7365,14 +7444,14 @@
       <c r="AD28" s="31"/>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B29" s="76">
+      <c r="B29" s="74">
         <v>100</v>
       </c>
       <c r="C29" s="6">
         <f t="shared" si="19"/>
         <v>1.568888888888889</v>
       </c>
-      <c r="D29" s="91">
+      <c r="D29" s="89">
         <f t="shared" si="20"/>
         <v>102.40000000000002</v>
       </c>
@@ -7397,10 +7476,10 @@
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
-      <c r="AA29" s="67" t="s">
+      <c r="AA29" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AB29" s="68">
+      <c r="AB29" s="67">
         <f>AE14</f>
         <v>5</v>
       </c>
@@ -7408,14 +7487,14 @@
       <c r="AD29" s="31"/>
     </row>
     <row r="30" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B30" s="76">
+      <c r="B30" s="74">
         <v>110</v>
       </c>
       <c r="C30" s="6">
         <f t="shared" si="19"/>
         <v>1.6727777777777779</v>
       </c>
-      <c r="D30" s="91">
+      <c r="D30" s="89">
         <f t="shared" si="20"/>
         <v>121.10000000000002</v>
       </c>
@@ -7438,10 +7517,10 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
-      <c r="AA30" s="67" t="s">
+      <c r="AA30" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AB30" s="68">
+      <c r="AB30" s="67">
         <f>AE13</f>
         <v>0</v>
       </c>
@@ -7449,21 +7528,21 @@
       <c r="AD30" s="31"/>
     </row>
     <row r="31" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B31" s="76">
+      <c r="B31" s="74">
         <v>114</v>
       </c>
       <c r="C31" s="6">
         <f t="shared" si="19"/>
         <v>1.7143333333333333</v>
       </c>
-      <c r="D31" s="91">
+      <c r="D31" s="89">
         <f t="shared" si="20"/>
         <v>128.57999999999998</v>
       </c>
-      <c r="AA31" s="67" t="s">
+      <c r="AA31" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="AB31" s="68">
+      <c r="AB31" s="67">
         <f>AB17/100</f>
         <v>221.53846153846152</v>
       </c>
@@ -7473,21 +7552,21 @@
       <c r="AO31" s="3"/>
     </row>
     <row r="32" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B32" s="76">
+      <c r="B32" s="74">
         <v>127.5</v>
       </c>
       <c r="C32" s="6">
         <f t="shared" si="19"/>
         <v>1.8545833333333333</v>
       </c>
-      <c r="D32" s="91">
+      <c r="D32" s="89">
         <f t="shared" si="20"/>
         <v>153.82499999999999</v>
       </c>
-      <c r="AA32" s="67" t="s">
+      <c r="AA32" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AB32" s="68">
+      <c r="AB32" s="67">
         <f>AJ22</f>
         <v>180</v>
       </c>
@@ -7496,21 +7575,21 @@
       <c r="AM32" s="3"/>
     </row>
     <row r="33" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="83">
+      <c r="B33" s="81">
         <v>136.4</v>
       </c>
       <c r="C33" s="6">
         <f t="shared" si="19"/>
         <v>1.9470444444444444</v>
       </c>
-      <c r="D33" s="91">
+      <c r="D33" s="89">
         <f t="shared" si="20"/>
         <v>170.46799999999999</v>
       </c>
-      <c r="AA33" s="67" t="s">
+      <c r="AA33" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="AB33" s="68">
+      <c r="AB33" s="67">
         <f>AJ21</f>
         <v>0</v>
       </c>
@@ -7519,31 +7598,31 @@
       <c r="AL33" s="3"/>
     </row>
     <row r="34" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="AA34" s="67" t="s">
+      <c r="AA34" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="AB34" s="68">
+      <c r="AB34" s="67">
         <f>AB22</f>
         <v>0</v>
       </c>
-      <c r="AC34" s="69">
+      <c r="AC34" s="68">
         <f>AB21</f>
         <v>7227.227639740272</v>
       </c>
-      <c r="AD34" s="70">
+      <c r="AD34" s="69">
         <f>AB20</f>
         <v>-475.97454575994487</v>
       </c>
     </row>
     <row r="35" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="AA35" s="67" t="s">
+      <c r="AA35" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="AB35" s="68">
+      <c r="AB35" s="67">
         <f>AB24</f>
         <v>-63471.680708889646</v>
       </c>
-      <c r="AC35" s="69">
+      <c r="AC35" s="68">
         <f>AB23</f>
         <v>16373.425300201903</v>
       </c>
@@ -7552,42 +7631,42 @@
       <c r="AK35" s="3"/>
     </row>
     <row r="36" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="AA36" s="67" t="s">
+      <c r="AA36" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="AB36" s="68">
+      <c r="AB36" s="92">
         <f>AK24</f>
-        <v>-5</v>
-      </c>
-      <c r="AC36" s="71">
+        <v>-17.719588605194332</v>
+      </c>
+      <c r="AC36" s="93">
         <f>AK23</f>
-        <v>15</v>
+        <v>17.543917721038866</v>
       </c>
       <c r="AD36" s="31"/>
     </row>
     <row r="37" spans="2:38" x14ac:dyDescent="0.3">
-      <c r="AA37" s="67" t="s">
+      <c r="AA37" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="AB37" s="68">
+      <c r="AB37" s="67">
         <f>AE23</f>
         <v>-3925.570398689204</v>
       </c>
-      <c r="AC37" s="72">
+      <c r="AC37" s="70">
         <f>AE22</f>
         <v>0.94199104022164515</v>
       </c>
       <c r="AD37" s="31"/>
     </row>
     <row r="38" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AA38" s="73" t="s">
+      <c r="AA38" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="AB38" s="74">
+      <c r="AB38" s="72">
         <f>AE21</f>
         <v>4180.4182204512181</v>
       </c>
-      <c r="AC38" s="75">
+      <c r="AC38" s="73">
         <f>AE20</f>
         <v>1.0602056822563426</v>
       </c>
@@ -7601,11 +7680,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO33"/>
+  <dimension ref="A1:AO38"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AH24" sqref="AH24"/>
+      <selection pane="bottomLeft" activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7630,7 +7709,7 @@
     <col min="22" max="22" width="8.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="25" width="6.109375" customWidth="1"/>
     <col min="27" max="27" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.33203125" customWidth="1"/>
+    <col min="28" max="28" width="10.6640625" customWidth="1"/>
     <col min="29" max="29" width="6.5546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.6640625" customWidth="1"/>
     <col min="31" max="31" width="8.5546875" bestFit="1" customWidth="1"/>
@@ -7645,28 +7724,28 @@
       <c r="A1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="85" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="86" t="s">
+      <c r="B1" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="86" t="s">
+      <c r="G1" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="I1" s="85" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="4" t="s">
@@ -7718,39 +7797,30 @@
         <f t="shared" ref="Y1:Y8" si="0">J1</f>
         <v>Charger Pwr, W</v>
       </c>
-      <c r="AA1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>50</v>
-      </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="B2" s="77">
+      <c r="B2" s="75">
         <v>1.1637222222222223</v>
       </c>
-      <c r="C2" s="88">
+      <c r="C2" s="86">
         <v>29.47000000000002</v>
       </c>
-      <c r="D2" s="88">
+      <c r="D2" s="86">
         <v>0.54</v>
       </c>
-      <c r="E2" s="88">
+      <c r="E2" s="86">
         <v>12.15</v>
       </c>
-      <c r="F2" s="88">
+      <c r="F2" s="86">
         <v>1.56</v>
       </c>
-      <c r="G2" s="88">
+      <c r="G2" s="86">
         <v>3810.7961637948006</v>
       </c>
-      <c r="H2" s="88">
+      <c r="H2" s="86">
         <v>8615</v>
       </c>
-      <c r="I2" s="89">
+      <c r="I2" s="87">
         <v>2.88</v>
       </c>
       <c r="J2" s="2">
@@ -7774,96 +7844,77 @@
         <v>116.07661056297157</v>
       </c>
       <c r="O2" s="3">
-        <f t="shared" ref="O2:P8" si="3">M2*60/$AB$2</f>
+        <f>M2*60/$AB$12</f>
         <v>7872.3706833287897</v>
       </c>
       <c r="P2" s="3">
-        <f t="shared" si="3"/>
+        <f>N2*60/$AB$12</f>
         <v>3482.2983168891469</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:R8" si="4">O2/$AB$7*100</f>
+        <f>O2/$AB$17*100</f>
         <v>35.535006556692458</v>
       </c>
       <c r="R2" s="3">
-        <f t="shared" si="4"/>
+        <f>P2/$AB$17*100</f>
         <v>15.7187076804024</v>
       </c>
       <c r="S2" s="3">
-        <f t="shared" ref="S2:S8" si="5">P2*$AE$10+$AE$11</f>
+        <f>P2*$AE$20+$AE$21</f>
         <v>7872.3706833287897</v>
       </c>
       <c r="T2" s="3">
-        <f t="shared" ref="T2:T8" si="6">K2</f>
+        <f t="shared" ref="T2:T8" si="3">K2</f>
         <v>29.47000000000002</v>
       </c>
       <c r="U2" s="3">
-        <f t="shared" ref="U2:U8" si="7">S2/$AB$7*100</f>
+        <f>S2/$AB$17*100</f>
         <v>35.535006556692458</v>
       </c>
       <c r="V2" s="3">
-        <f t="shared" ref="V2:V8" si="8">$AB$13*LN(C2)+$AB$14</f>
+        <f>$AB$23*LN(C2)+$AB$24</f>
         <v>7254.3033712821489</v>
       </c>
       <c r="W2" s="3">
-        <f t="shared" ref="W2:W8" si="9">D2*D2*$AB$10+D2*$AB$11+$AB$12</f>
+        <f>D2*D2*$AB$20+D2*$AB$21+$AB$22</f>
         <v>3895.0045670565887</v>
       </c>
       <c r="X2" s="3">
-        <f t="shared" ref="X2:X8" si="10">W2/$AB$7*100</f>
+        <f>W2/$AB$17*100</f>
         <v>17.581617837408213</v>
       </c>
       <c r="Y2" s="4">
         <f t="shared" si="0"/>
         <v>18.954000000000001</v>
       </c>
-      <c r="AA2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="18">
-        <v>2</v>
-      </c>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH2" s="28"/>
-      <c r="AI2" s="28"/>
-      <c r="AJ2" s="28"/>
-      <c r="AK2" s="28"/>
-      <c r="AL2" s="29"/>
     </row>
     <row r="3" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="80">
+      <c r="B3" s="78">
         <v>1.2052777777777779</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="74">
         <v>36.950000000000017</v>
       </c>
-      <c r="D3" s="76">
+      <c r="D3" s="74">
         <v>0.68</v>
       </c>
-      <c r="E3" s="76">
+      <c r="E3" s="74">
         <v>12.14</v>
       </c>
-      <c r="F3" s="76">
+      <c r="F3" s="74">
         <v>1.9</v>
       </c>
-      <c r="G3" s="76">
+      <c r="G3" s="74">
         <v>3247.7925769058029</v>
       </c>
-      <c r="H3" s="76">
+      <c r="H3" s="74">
         <v>6290</v>
       </c>
-      <c r="I3" s="81">
+      <c r="I3" s="79">
         <v>4.0199999999999996</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J7" si="11">E3*F3</f>
+        <f t="shared" ref="J3:J7" si="4">E3*F3</f>
         <v>23.065999999999999</v>
       </c>
       <c r="K3" s="1">
@@ -7871,7 +7922,7 @@
         <v>36.950000000000017</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L8" si="12">LN(K3)</f>
+        <f t="shared" ref="L3:L8" si="5">LN(K3)</f>
         <v>3.609565647394211</v>
       </c>
       <c r="M3" s="3">
@@ -7883,97 +7934,77 @@
         <v>158.98251192368841</v>
       </c>
       <c r="O3" s="3">
+        <f>M3*60/$AB$12</f>
+        <v>9237.0430960776539</v>
+      </c>
+      <c r="P3" s="3">
+        <f>N3*60/$AB$12</f>
+        <v>4769.4753577106521</v>
+      </c>
+      <c r="Q3" s="3">
+        <f>O3/$AB$17*100</f>
+        <v>41.694986197572746</v>
+      </c>
+      <c r="R3" s="3">
+        <f>P3/$AB$17*100</f>
+        <v>21.528881822999473</v>
+      </c>
+      <c r="S3" s="3">
+        <f>P3*$AE$20+$AE$21</f>
+        <v>9237.0430960776539</v>
+      </c>
+      <c r="T3" s="3">
         <f t="shared" si="3"/>
-        <v>9237.0430960776539</v>
-      </c>
-      <c r="P3" s="3">
-        <f t="shared" si="3"/>
-        <v>4769.4753577106521</v>
-      </c>
-      <c r="Q3" s="3">
-        <f t="shared" si="4"/>
+        <v>36.950000000000017</v>
+      </c>
+      <c r="U3" s="3">
+        <f>S3/$AB$17*100</f>
         <v>41.694986197572746</v>
       </c>
-      <c r="R3" s="3">
-        <f t="shared" si="4"/>
-        <v>21.528881822999473</v>
-      </c>
-      <c r="S3" s="3">
-        <f t="shared" si="5"/>
-        <v>9237.0430960776539</v>
-      </c>
-      <c r="T3" s="3">
-        <f t="shared" si="6"/>
-        <v>36.950000000000017</v>
-      </c>
-      <c r="U3" s="3">
-        <f t="shared" si="7"/>
-        <v>41.694986197572746</v>
-      </c>
       <c r="V3" s="3">
-        <f t="shared" si="8"/>
+        <f>$AB$23*LN(C3)+$AB$24</f>
         <v>9298.3552461146719</v>
       </c>
       <c r="W3" s="3">
-        <f t="shared" si="9"/>
+        <f>D3*D3*$AB$20+D3*$AB$21+$AB$22</f>
         <v>4863.4075129077619</v>
       </c>
       <c r="X3" s="3">
-        <f t="shared" si="10"/>
+        <f>W3/$AB$17*100</f>
         <v>21.952881134653094</v>
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
         <v>23.065999999999999</v>
       </c>
-      <c r="AA3" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB3" s="20">
-        <v>4800</v>
-      </c>
-      <c r="AD3" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="AH3" s="30"/>
-      <c r="AI3" s="30"/>
-      <c r="AJ3" s="30"/>
-      <c r="AK3" s="30"/>
-      <c r="AL3" s="31"/>
     </row>
-    <row r="4" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="80">
+    <row r="4" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="78">
         <v>1.3299444444444444</v>
       </c>
-      <c r="C4" s="76">
+      <c r="C4" s="74">
         <v>59.389999999999986</v>
       </c>
-      <c r="D4" s="76">
+      <c r="D4" s="74">
         <v>1.18</v>
       </c>
-      <c r="E4" s="76">
+      <c r="E4" s="74">
         <v>12.07</v>
       </c>
-      <c r="F4" s="76">
+      <c r="F4" s="74">
         <v>3.66</v>
       </c>
-      <c r="G4" s="76">
+      <c r="G4" s="74">
         <v>2314.9259570838622</v>
       </c>
-      <c r="H4" s="76">
+      <c r="H4" s="74">
         <v>3623</v>
       </c>
-      <c r="I4" s="81">
+      <c r="I4" s="79">
         <v>7.4</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>44.176200000000001</v>
       </c>
       <c r="K4" s="1">
@@ -7981,7 +8012,7 @@
         <v>59.389999999999986</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>4.0841258620277685</v>
       </c>
       <c r="M4" s="3">
@@ -7993,97 +8024,77 @@
         <v>276.01435274634281</v>
       </c>
       <c r="O4" s="3">
+        <f>M4*60/$AB$12</f>
+        <v>12959.377775430594</v>
+      </c>
+      <c r="P4" s="3">
+        <f>N4*60/$AB$12</f>
+        <v>8280.4305823902851</v>
+      </c>
+      <c r="Q4" s="3">
+        <f>O4/$AB$17*100</f>
+        <v>58.497191347429769</v>
+      </c>
+      <c r="R4" s="3">
+        <f>P4/$AB$17*100</f>
+        <v>37.376943601067261</v>
+      </c>
+      <c r="S4" s="3">
+        <f>P4*$AE$20+$AE$21</f>
+        <v>12959.377775430594</v>
+      </c>
+      <c r="T4" s="3">
         <f t="shared" si="3"/>
-        <v>12959.377775430594</v>
-      </c>
-      <c r="P4" s="3">
-        <f t="shared" si="3"/>
-        <v>8280.4305823902851</v>
-      </c>
-      <c r="Q4" s="3">
-        <f t="shared" si="4"/>
+        <v>59.389999999999986</v>
+      </c>
+      <c r="U4" s="3">
+        <f>S4/$AB$17*100</f>
         <v>58.497191347429769</v>
       </c>
-      <c r="R4" s="3">
-        <f t="shared" si="4"/>
-        <v>37.376943601067261</v>
-      </c>
-      <c r="S4" s="3">
-        <f t="shared" si="5"/>
-        <v>12959.377775430594</v>
-      </c>
-      <c r="T4" s="3">
-        <f t="shared" si="6"/>
-        <v>59.389999999999986</v>
-      </c>
-      <c r="U4" s="3">
-        <f t="shared" si="7"/>
-        <v>58.497191347429769</v>
-      </c>
       <c r="V4" s="3">
-        <f t="shared" si="8"/>
+        <f>$AB$23*LN(C4)+$AB$24</f>
         <v>13586.844885279916</v>
       </c>
       <c r="W4" s="3">
-        <f t="shared" si="9"/>
+        <f>D4*D4*$AB$20+D4*$AB$21+$AB$22</f>
         <v>8182.7859228288444</v>
       </c>
       <c r="X4" s="3">
-        <f t="shared" si="10"/>
+        <f>W4/$AB$17*100</f>
         <v>36.936186457213537</v>
       </c>
       <c r="Y4" s="4">
         <f t="shared" si="0"/>
         <v>44.176200000000001</v>
       </c>
-      <c r="AA4" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB4" s="22">
-        <v>12</v>
-      </c>
-      <c r="AD4" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE4" s="27">
-        <v>5</v>
-      </c>
-      <c r="AG4" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="AH4" s="32"/>
-      <c r="AI4" s="33"/>
-      <c r="AJ4" s="33"/>
-      <c r="AK4" s="32"/>
-      <c r="AL4" s="34"/>
     </row>
     <row r="5" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="80">
+      <c r="B5" s="78">
         <v>1.4442222222222223</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="74">
         <v>79.960000000000008</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="74">
         <v>1.57</v>
       </c>
-      <c r="E5" s="76">
+      <c r="E5" s="74">
         <v>11.96</v>
       </c>
-      <c r="F5" s="76">
+      <c r="F5" s="74">
         <v>6.51</v>
       </c>
-      <c r="G5" s="76">
+      <c r="G5" s="74">
         <v>1890.4108937169444</v>
       </c>
-      <c r="H5" s="76">
+      <c r="H5" s="74">
         <v>2721</v>
       </c>
-      <c r="I5" s="81">
+      <c r="I5" s="79">
         <v>9.5</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>77.8596</v>
       </c>
       <c r="K5" s="1">
@@ -8091,7 +8102,7 @@
         <v>79.960000000000008</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>4.3815265096321996</v>
       </c>
       <c r="M5" s="3">
@@ -8103,43 +8114,43 @@
         <v>367.51194413818456</v>
       </c>
       <c r="O5" s="3">
+        <f>M5*60/$AB$12</f>
+        <v>15869.565764622583</v>
+      </c>
+      <c r="P5" s="3">
+        <f>N5*60/$AB$12</f>
+        <v>11025.358324145536</v>
+      </c>
+      <c r="Q5" s="3">
+        <f>O5/$AB$17*100</f>
+        <v>71.633456576421381</v>
+      </c>
+      <c r="R5" s="3">
+        <f>P5/$AB$17*100</f>
+        <v>49.76724243537916</v>
+      </c>
+      <c r="S5" s="3">
+        <f>P5*$AE$20+$AE$21</f>
+        <v>15869.565764622583</v>
+      </c>
+      <c r="T5" s="3">
         <f t="shared" si="3"/>
-        <v>15869.565764622583</v>
-      </c>
-      <c r="P5" s="3">
-        <f t="shared" si="3"/>
-        <v>11025.358324145536</v>
-      </c>
-      <c r="Q5" s="3">
-        <f t="shared" si="4"/>
+        <v>79.960000000000008</v>
+      </c>
+      <c r="U5" s="3">
+        <f>S5/$AB$17*100</f>
         <v>71.633456576421381</v>
       </c>
-      <c r="R5" s="3">
-        <f t="shared" si="4"/>
-        <v>49.76724243537916</v>
-      </c>
-      <c r="S5" s="3">
-        <f t="shared" si="5"/>
-        <v>15869.565764622583</v>
-      </c>
-      <c r="T5" s="3">
-        <f t="shared" si="6"/>
-        <v>79.960000000000008</v>
-      </c>
-      <c r="U5" s="3">
-        <f t="shared" si="7"/>
-        <v>71.633456576421381</v>
-      </c>
       <c r="V5" s="3">
-        <f t="shared" si="8"/>
+        <f>$AB$23*LN(C5)+$AB$24</f>
         <v>16274.384962607019</v>
       </c>
       <c r="W5" s="3">
-        <f t="shared" si="9"/>
+        <f>D5*D5*$AB$20+D5*$AB$21+$AB$22</f>
         <v>10620.908743264476</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="10"/>
+        <f>W5/$AB$17*100</f>
         <v>47.941601966124367</v>
       </c>
       <c r="Y5" s="4">
@@ -8147,33 +8158,33 @@
         <v>77.8596</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="80">
+    <row r="6" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="78">
         <v>1.5169444444444444</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="74">
         <v>93.05</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="74">
         <v>1.88</v>
       </c>
-      <c r="E6" s="76">
+      <c r="E6" s="74">
         <v>11.86</v>
       </c>
-      <c r="F6" s="76">
+      <c r="F6" s="74">
         <v>8.49</v>
       </c>
-      <c r="G6" s="76">
+      <c r="G6" s="74">
         <v>1735.553038041201</v>
       </c>
-      <c r="H6" s="76">
+      <c r="H6" s="74">
         <v>2427</v>
       </c>
-      <c r="I6" s="81">
+      <c r="I6" s="79">
         <v>10.5</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>100.6914</v>
       </c>
       <c r="K6" s="1">
@@ -8181,7 +8192,7 @@
         <v>93.05</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>4.5331369830882595</v>
       </c>
       <c r="M6" s="3">
@@ -8193,83 +8204,77 @@
         <v>412.03131437989288</v>
       </c>
       <c r="O6" s="3">
+        <f>M6*60/$AB$12</f>
+        <v>17285.556443644575</v>
+      </c>
+      <c r="P6" s="3">
+        <f>N6*60/$AB$12</f>
+        <v>12360.939431396786</v>
+      </c>
+      <c r="Q6" s="3">
+        <f>O6/$AB$17*100</f>
+        <v>78.025081169228997</v>
+      </c>
+      <c r="R6" s="3">
+        <f>P6/$AB$17*100</f>
+        <v>55.795907155610493</v>
+      </c>
+      <c r="S6" s="3">
+        <f>P6*$AE$20+$AE$21</f>
+        <v>17285.556443644575</v>
+      </c>
+      <c r="T6" s="3">
         <f t="shared" si="3"/>
-        <v>17285.556443644575</v>
-      </c>
-      <c r="P6" s="3">
-        <f t="shared" si="3"/>
-        <v>12360.939431396786</v>
-      </c>
-      <c r="Q6" s="3">
-        <f t="shared" si="4"/>
+        <v>93.05</v>
+      </c>
+      <c r="U6" s="3">
+        <f>S6/$AB$17*100</f>
         <v>78.025081169228997</v>
       </c>
-      <c r="R6" s="3">
-        <f t="shared" si="4"/>
-        <v>55.795907155610493</v>
-      </c>
-      <c r="S6" s="3">
-        <f t="shared" si="5"/>
-        <v>17285.556443644575</v>
-      </c>
-      <c r="T6" s="3">
-        <f t="shared" si="6"/>
-        <v>93.05</v>
-      </c>
-      <c r="U6" s="3">
-        <f t="shared" si="7"/>
-        <v>78.025081169228997</v>
-      </c>
       <c r="V6" s="3">
-        <f t="shared" si="8"/>
+        <f>$AB$23*LN(C6)+$AB$24</f>
         <v>17644.453342880533</v>
       </c>
       <c r="W6" s="3">
-        <f t="shared" si="9"/>
+        <f>D6*D6*$AB$20+D6*$AB$21+$AB$22</f>
         <v>12464.506405406451</v>
       </c>
       <c r="X6" s="3">
-        <f t="shared" si="10"/>
+        <f>W6/$AB$17*100</f>
         <v>56.263396968848568</v>
       </c>
       <c r="Y6" s="4">
         <f t="shared" si="0"/>
         <v>100.6914</v>
       </c>
-      <c r="AA6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="7" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="80">
+    <row r="7" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="78">
         <v>1.6208333333333333</v>
       </c>
-      <c r="C7" s="76">
+      <c r="C7" s="74">
         <v>111.75</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="74">
         <v>2.2400000000000002</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="74">
         <v>11.55</v>
       </c>
-      <c r="F7" s="76">
+      <c r="F7" s="74">
         <v>13.48</v>
       </c>
-      <c r="G7" s="76">
+      <c r="G7" s="74">
         <v>1544.1739275824405</v>
       </c>
-      <c r="H7" s="76">
+      <c r="H7" s="74">
         <v>2086</v>
       </c>
-      <c r="I7" s="81">
+      <c r="I7" s="79">
         <v>12.4</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="4"/>
         <v>155.69400000000002</v>
       </c>
       <c r="K7" s="1">
@@ -8277,7 +8282,7 @@
         <v>111.75</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>4.7162642334936784</v>
       </c>
       <c r="M7" s="3">
@@ -8289,94 +8294,69 @@
         <v>479.38638542665387</v>
       </c>
       <c r="O7" s="3">
+        <f>M7*60/$AB$12</f>
+        <v>19427.863315221246</v>
+      </c>
+      <c r="P7" s="3">
+        <f>N7*60/$AB$12</f>
+        <v>14381.591562799616</v>
+      </c>
+      <c r="Q7" s="3">
+        <f>O7/$AB$17*100</f>
+        <v>87.695216353429245</v>
+      </c>
+      <c r="R7" s="3">
+        <f>P7/$AB$17*100</f>
+        <v>64.916906359859382</v>
+      </c>
+      <c r="S7" s="3">
+        <f>P7*$AE$20+$AE$21</f>
+        <v>19427.863315221246</v>
+      </c>
+      <c r="T7" s="3">
         <f t="shared" si="3"/>
-        <v>19427.863315221246</v>
-      </c>
-      <c r="P7" s="3">
-        <f t="shared" si="3"/>
-        <v>14381.591562799616</v>
-      </c>
-      <c r="Q7" s="3">
-        <f t="shared" si="4"/>
+        <v>111.75</v>
+      </c>
+      <c r="U7" s="3">
+        <f>S7/$AB$17*100</f>
         <v>87.695216353429245</v>
       </c>
-      <c r="R7" s="3">
-        <f t="shared" si="4"/>
-        <v>64.916906359859382</v>
-      </c>
-      <c r="S7" s="3">
-        <f t="shared" si="5"/>
-        <v>19427.863315221246</v>
-      </c>
-      <c r="T7" s="3">
-        <f t="shared" si="6"/>
-        <v>111.75</v>
-      </c>
-      <c r="U7" s="3">
-        <f t="shared" si="7"/>
-        <v>87.695216353429245</v>
-      </c>
       <c r="V7" s="3">
-        <f t="shared" si="8"/>
+        <f>$AB$23*LN(C7)+$AB$24</f>
         <v>19299.331463286977</v>
       </c>
       <c r="W7" s="3">
-        <f t="shared" si="9"/>
+        <f>D7*D7*$AB$20+D7*$AB$21+$AB$22</f>
         <v>14500.533861250384</v>
       </c>
       <c r="X7" s="3">
-        <f t="shared" si="10"/>
+        <f>W7/$AB$17*100</f>
         <v>65.4537986792552</v>
       </c>
       <c r="Y7" s="4">
         <f t="shared" si="0"/>
         <v>155.69400000000002</v>
       </c>
-      <c r="AA7" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="AB7" s="40">
-        <f>AB3*AB4/AC7</f>
-        <v>22153.846153846152</v>
-      </c>
-      <c r="AC7" s="41">
-        <v>2.6</v>
-      </c>
-      <c r="AD7" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE7" s="42"/>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="35">
-        <v>210</v>
-      </c>
-      <c r="AH7" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI7" s="37"/>
-      <c r="AJ7" s="36"/>
-      <c r="AK7" s="36"/>
-      <c r="AL7" s="38"/>
     </row>
     <row r="8" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="82">
+      <c r="B8" s="80">
         <v>1.7766666666666666</v>
       </c>
-      <c r="C8" s="83">
+      <c r="C8" s="81">
         <v>139.79999999999998</v>
       </c>
-      <c r="D8" s="83">
+      <c r="D8" s="81">
         <v>2.68</v>
       </c>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83">
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81">
         <v>1361.8412878381814</v>
       </c>
-      <c r="H8" s="83">
+      <c r="H8" s="81">
         <v>1782</v>
       </c>
-      <c r="I8" s="84">
+      <c r="I8" s="82">
         <v>14.4</v>
       </c>
       <c r="J8" s="2"/>
@@ -8385,7 +8365,7 @@
         <v>139.79999999999998</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="5"/>
         <v>4.9402128297997097</v>
       </c>
       <c r="M8" s="3">
@@ -8397,62 +8377,51 @@
         <v>561.16722783389457</v>
       </c>
       <c r="O8" s="3">
+        <f>M8*60/$AB$12</f>
+        <v>22028.998729817256</v>
+      </c>
+      <c r="P8" s="3">
+        <f>N8*60/$AB$12</f>
+        <v>16835.016835016839</v>
+      </c>
+      <c r="Q8" s="3">
+        <f>O8/$AB$17*100</f>
+        <v>99.436452599869568</v>
+      </c>
+      <c r="R8" s="3">
+        <f>P8/$AB$17*100</f>
+        <v>75.991395435839905</v>
+      </c>
+      <c r="S8" s="3">
+        <f>P8*$AE$20+$AE$21</f>
+        <v>22028.99872981726</v>
+      </c>
+      <c r="T8" s="3">
         <f t="shared" si="3"/>
-        <v>22028.998729817256</v>
-      </c>
-      <c r="P8" s="3">
-        <f t="shared" si="3"/>
-        <v>16835.016835016839</v>
-      </c>
-      <c r="Q8" s="3">
-        <f t="shared" si="4"/>
-        <v>99.436452599869568</v>
-      </c>
-      <c r="R8" s="3">
-        <f t="shared" si="4"/>
-        <v>75.991395435839905</v>
-      </c>
-      <c r="S8" s="3">
-        <f t="shared" si="5"/>
-        <v>22028.99872981726</v>
-      </c>
-      <c r="T8" s="3">
-        <f t="shared" si="6"/>
         <v>139.79999999999998</v>
       </c>
       <c r="U8" s="3">
-        <f t="shared" si="7"/>
+        <f>S8/$AB$17*100</f>
         <v>99.436452599869583</v>
       </c>
       <c r="V8" s="3">
-        <f t="shared" si="8"/>
+        <f>$AB$23*LN(C8)+$AB$24</f>
         <v>21323.102536691451</v>
       </c>
       <c r="W8" s="3">
-        <f t="shared" si="9"/>
+        <f>D8*D8*$AB$20+D8*$AB$21+$AB$22</f>
         <v>16835.887969335279</v>
       </c>
       <c r="X8" s="3">
-        <f t="shared" si="10"/>
+        <f>W8/$AB$17*100</f>
         <v>75.995327639360639</v>
       </c>
       <c r="Y8" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AF8" s="8"/>
-      <c r="AG8" s="8"/>
-      <c r="AI8" s="8"/>
-      <c r="AJ8" s="8"/>
     </row>
-    <row r="9" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AA9" t="s">
-        <v>56</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>54</v>
-      </c>
-    </row>
+    <row r="9" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="6"/>
@@ -8476,35 +8445,8 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
-      <c r="AA10" s="50" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB10" s="51">
-        <f>INDEX(LINEST($P$2:$P$8,$D$2:$D$8^{1,2},FALSE,FALSE),1)</f>
-        <v>-435.01106108560458</v>
-      </c>
-      <c r="AC10" s="28"/>
-      <c r="AD10" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE10" s="18">
-        <f>CalArduino!AE20</f>
-        <v>1.0602056822563426</v>
-      </c>
-      <c r="AF10" s="8"/>
-      <c r="AG10" s="17"/>
-      <c r="AH10" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI10" s="28"/>
-      <c r="AJ10" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK10" s="29" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="11" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -8517,13 +8459,13 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="P11" s="3" t="s">
+      <c r="Q11" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
@@ -8533,41 +8475,25 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-      <c r="AA11" s="44"/>
-      <c r="AB11" s="54">
-        <f>INDEX(LINEST($P$2:$P$8,$D$2:$D$8^{1,2},FALSE,FALSE),2)</f>
-        <v>7447.8773934613901</v>
-      </c>
-      <c r="AC11" s="30"/>
-      <c r="AD11" s="45"/>
-      <c r="AE11" s="20">
-        <f>CalArduino!AE21</f>
-        <v>4180.4182204512181</v>
-      </c>
-      <c r="AF11" s="8"/>
-      <c r="AG11" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH11" s="59">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ11" s="60">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="61">
-        <v>-5</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>59</v>
+      <c r="AA11" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -8584,7 +8510,7 @@
         <v>7872.3706833287897</v>
       </c>
       <c r="Q12" s="3">
-        <f>P12/60*$AB$2</f>
+        <f>P12/60*$AB$12</f>
         <v>262.41235611095965</v>
       </c>
       <c r="R12" s="3">
@@ -8598,39 +8524,33 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
-      <c r="AA12" s="44"/>
-      <c r="AB12" s="45">
-        <f>INDEX(LINEST($P$2:$P$8,$D$2:$D$8^{1,2},FALSE,FALSE),3)</f>
-        <v>0</v>
-      </c>
-      <c r="AC12" s="30"/>
-      <c r="AD12" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE12" s="20">
-        <f>CalArduino!AE22</f>
-        <v>0.94199104022164515</v>
-      </c>
-      <c r="AG12" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH12" s="59">
-        <v>3.3</v>
-      </c>
-      <c r="AI12" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="AJ12" s="60">
-        <v>180</v>
-      </c>
-      <c r="AK12" s="61">
-        <v>70</v>
-      </c>
+      <c r="AA12" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB12" s="18">
+        <v>2</v>
+      </c>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH12" s="28"/>
+      <c r="AI12" s="28"/>
+      <c r="AJ12" s="28"/>
+      <c r="AK12" s="28"/>
+      <c r="AL12" s="29"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -8647,11 +8567,11 @@
         <v>9237.0430960776539</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" ref="Q13:Q18" si="13">P13/60*$AB$2</f>
+        <f>P13/60*$AB$12</f>
         <v>307.90143653592179</v>
       </c>
       <c r="R13" s="3">
-        <f t="shared" ref="R13:R18" si="14">1/Q13/0.000001</f>
+        <f t="shared" ref="R13:R18" si="6">1/Q13/0.000001</f>
         <v>3247.7925769058029</v>
       </c>
       <c r="S13" s="3"/>
@@ -8661,34 +8581,34 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
-      <c r="AA13" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB13" s="55">
-        <f>INDEX(LINEST($S$2:$S$8,$L$2:$L$8),1)</f>
-        <v>9036.7660560772038</v>
-      </c>
-      <c r="AC13" s="30"/>
-      <c r="AD13" s="45"/>
-      <c r="AE13" s="20">
-        <f>CalArduino!AE23</f>
-        <v>-3925.570398689204</v>
-      </c>
-      <c r="AG13" s="19"/>
-      <c r="AH13" s="30" t="s">
-        <v>60</v>
-      </c>
+      <c r="AA13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB13" s="20">
+        <v>4800</v>
+      </c>
+      <c r="AD13" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE13" s="25">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH13" s="30"/>
       <c r="AI13" s="30"/>
-      <c r="AJ13" s="62"/>
-      <c r="AK13" s="63">
-        <f>(AK12-AK11)/(AH12-AH11)</f>
-        <v>22.72727272727273</v>
-      </c>
+      <c r="AJ13" s="30"/>
+      <c r="AK13" s="30"/>
+      <c r="AL13" s="31"/>
     </row>
     <row r="14" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -8705,42 +8625,38 @@
         <v>12959.377775430594</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="13"/>
+        <f>P14/60*$AB$12</f>
         <v>431.97925918101981</v>
       </c>
       <c r="R14" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>2314.9259570838622</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
-      <c r="U14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="V14" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="W14" s="12"/>
-      <c r="X14" s="12"/>
       <c r="Y14" s="3"/>
-      <c r="AA14" s="56"/>
-      <c r="AB14" s="57">
-        <f>INDEX(LINEST($S$2:$S$8,$L$2:$L$8),2)</f>
-        <v>-23320.445073439671</v>
-      </c>
-      <c r="AC14" s="32"/>
-      <c r="AD14" s="32"/>
-      <c r="AE14" s="34"/>
-      <c r="AG14" s="19"/>
-      <c r="AH14" s="30"/>
-      <c r="AI14" s="30"/>
-      <c r="AJ14" s="62"/>
-      <c r="AK14" s="63">
-        <f>AK12-AK13*(AH12-AH11)</f>
-        <v>-5</v>
-      </c>
+      <c r="AA14" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB14" s="22">
+        <v>12</v>
+      </c>
+      <c r="AD14" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE14" s="27">
+        <v>5</v>
+      </c>
+      <c r="AG14" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="33"/>
+      <c r="AJ14" s="33"/>
+      <c r="AK14" s="32"/>
+      <c r="AL14" s="34"/>
     </row>
-    <row r="15" spans="1:38" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:38" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -8760,32 +8676,16 @@
         <v>15869.565764622583</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="13"/>
+        <f>P15/60*$AB$12</f>
         <v>528.98552548741941</v>
       </c>
       <c r="R15" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>1890.4108937169444</v>
       </c>
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
       <c r="Y15" s="3"/>
-      <c r="AD15" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="32"/>
-      <c r="AI15" s="32"/>
-      <c r="AJ15" s="48"/>
-      <c r="AK15" s="49" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="16" spans="1:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5"/>
@@ -8807,29 +8707,24 @@
         <v>17285.556443644575</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="13"/>
+        <f>P16/60*$AB$12</f>
         <v>576.18521478815251</v>
       </c>
       <c r="R16" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>1735.553038041201</v>
       </c>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="W16" s="16"/>
-      <c r="X16" s="16"/>
       <c r="Y16" s="3"/>
-      <c r="AA16" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB16" s="5"/>
-      <c r="AC16" s="5"/>
+      <c r="AA16" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -8849,11 +8744,11 @@
         <v>19427.863315221246</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="13"/>
+        <f>P17/60*$AB$12</f>
         <v>647.59544384070819</v>
       </c>
       <c r="R17" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>1544.1739275824405</v>
       </c>
       <c r="S17" s="3"/>
@@ -8862,15 +8757,31 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
       <c r="Y17" s="3"/>
-      <c r="AA17" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB17" s="90">
-        <f>AH12</f>
-        <v>3.3</v>
-      </c>
-      <c r="AC17" s="66"/>
-      <c r="AD17" s="29"/>
+      <c r="AA17" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB17" s="40">
+        <f>AB13*AB14/AC17</f>
+        <v>22153.846153846152</v>
+      </c>
+      <c r="AC17" s="41">
+        <v>2.6</v>
+      </c>
+      <c r="AD17" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE17" s="42"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="35">
+        <v>210</v>
+      </c>
+      <c r="AH17" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI17" s="37"/>
+      <c r="AJ17" s="36"/>
+      <c r="AK17" s="36"/>
+      <c r="AL17" s="38"/>
     </row>
     <row r="18" spans="2:41" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
@@ -8892,11 +8803,11 @@
         <v>22028.99872981726</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="13"/>
+        <f>P18/60*$AB$12</f>
         <v>734.29995766057539</v>
       </c>
       <c r="R18" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="6"/>
         <v>1361.8412878381814</v>
       </c>
       <c r="S18" s="3"/>
@@ -8906,17 +8817,12 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
       <c r="Y18" s="3"/>
-      <c r="AA18" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB18" s="68">
-        <f>AH11</f>
-        <v>0</v>
-      </c>
-      <c r="AC18" s="46"/>
-      <c r="AD18" s="31"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="8"/>
     </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -8938,37 +8844,77 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
-      <c r="AA19" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB19" s="68">
-        <f>AE4</f>
-        <v>5</v>
-      </c>
-      <c r="AC19" s="30"/>
-      <c r="AD19" s="31"/>
+      <c r="AA19" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="AA20" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB20" s="68">
-        <f>AE3</f>
-        <v>0</v>
-      </c>
-      <c r="AC20" s="30"/>
-      <c r="AD20" s="31"/>
+    <row r="20" spans="2:41" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="AA20" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB20" s="51">
+        <f>INDEX(LINEST($P$2:$P$8,$D$2:$D$8^{1,2},FALSE,FALSE),1)</f>
+        <v>-435.01106108560458</v>
+      </c>
+      <c r="AC20" s="28"/>
+      <c r="AD20" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE20" s="53">
+        <f>CalArduino!AE20</f>
+        <v>1.0602056822563426</v>
+      </c>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="17"/>
+      <c r="AH20" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI20" s="28"/>
+      <c r="AJ20" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK20" s="29" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="AA21" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB21" s="68">
-        <f>AB7/100</f>
-        <v>221.53846153846152</v>
+      <c r="AA21" s="44"/>
+      <c r="AB21" s="54">
+        <f>INDEX(LINEST($P$2:$P$8,$D$2:$D$8^{1,2},FALSE,FALSE),2)</f>
+        <v>7447.8773934613901</v>
       </c>
       <c r="AC21" s="30"/>
-      <c r="AD21" s="31"/>
+      <c r="AD21" s="45"/>
+      <c r="AE21" s="47">
+        <f>CalArduino!AE21</f>
+        <v>4180.4182204512181</v>
+      </c>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH21" s="59">
+        <v>0</v>
+      </c>
+      <c r="AI21" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ21" s="60">
+        <v>0</v>
+      </c>
+      <c r="AK21" s="90">
+        <f>AE23/AB17*100</f>
+        <v>-17.719588605194325</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="22" spans="2:41" x14ac:dyDescent="0.3">
       <c r="C22" s="6"/>
@@ -8994,17 +8940,34 @@
       <c r="W22" s="10"/>
       <c r="X22" s="10"/>
       <c r="Y22" s="10"/>
-      <c r="AA22" s="67" t="s">
+      <c r="AA22" s="44"/>
+      <c r="AB22" s="45">
+        <f>INDEX(LINEST($P$2:$P$8,$D$2:$D$8^{1,2},FALSE,FALSE),3)</f>
+        <v>0</v>
+      </c>
+      <c r="AC22" s="30"/>
+      <c r="AD22" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE22" s="47">
+        <f>CalArduino!AE22</f>
+        <v>0.94199104022164515</v>
+      </c>
+      <c r="AG22" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="AH22" s="59">
+        <v>3.3</v>
+      </c>
+      <c r="AI22" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="AB22" s="68">
-        <f>AJ12</f>
+      <c r="AJ22" s="60">
         <v>180</v>
       </c>
-      <c r="AC22" s="30"/>
-      <c r="AD22" s="31"/>
-      <c r="AM22" s="3"/>
-      <c r="AN22" s="3"/>
+      <c r="AK22" s="61">
+        <v>70</v>
+      </c>
       <c r="AO22" s="3"/>
     </row>
     <row r="23" spans="2:41" x14ac:dyDescent="0.3">
@@ -9031,18 +8994,31 @@
       <c r="W23" s="10"/>
       <c r="X23" s="10"/>
       <c r="Y23" s="10"/>
-      <c r="AA23" s="67" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB23" s="68">
-        <f>AJ11</f>
-        <v>0</v>
+      <c r="AA23" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB23" s="55">
+        <f>INDEX(LINEST($S$2:$S$8,$L$2:$L$8),1)</f>
+        <v>9036.7660560772038</v>
       </c>
       <c r="AC23" s="30"/>
-      <c r="AD23" s="31"/>
-      <c r="AL23" s="3"/>
+      <c r="AD23" s="45"/>
+      <c r="AE23" s="47">
+        <f>CalArduino!AE23</f>
+        <v>-3925.570398689204</v>
+      </c>
+      <c r="AG23" s="19"/>
+      <c r="AH23" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI23" s="30"/>
+      <c r="AJ23" s="62"/>
+      <c r="AK23" s="90">
+        <f>(AK22-AK21)/(AH22-AH21)</f>
+        <v>26.581693516725558</v>
+      </c>
     </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -9066,23 +9042,24 @@
       <c r="W24" s="10"/>
       <c r="X24" s="10"/>
       <c r="Y24" s="10"/>
-      <c r="AA24" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB24" s="68">
-        <f>AB12</f>
-        <v>0</v>
-      </c>
-      <c r="AC24" s="69">
-        <f>AB11</f>
-        <v>7447.8773934613901</v>
-      </c>
-      <c r="AD24" s="70">
-        <f>AB10</f>
-        <v>-435.01106108560458</v>
+      <c r="AA24" s="56"/>
+      <c r="AB24" s="57">
+        <f>INDEX(LINEST($S$2:$S$8,$L$2:$L$8),2)</f>
+        <v>-23320.445073439671</v>
+      </c>
+      <c r="AC24" s="32"/>
+      <c r="AD24" s="32"/>
+      <c r="AE24" s="34"/>
+      <c r="AG24" s="19"/>
+      <c r="AH24" s="30"/>
+      <c r="AI24" s="30"/>
+      <c r="AJ24" s="62"/>
+      <c r="AK24" s="90">
+        <f>AK22-AK23*(AH22-AH21)</f>
+        <v>-17.719588605194332</v>
       </c>
     </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -9106,30 +9083,23 @@
       <c r="W25" s="10"/>
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
-      <c r="AA25" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB25" s="68">
-        <f>AB14</f>
-        <v>-23320.445073439671</v>
-      </c>
-      <c r="AC25" s="69">
-        <f>AB13</f>
-        <v>9036.7660560772038</v>
-      </c>
-      <c r="AD25" s="31"/>
-      <c r="AJ25" s="3"/>
-      <c r="AK25" s="3"/>
+      <c r="AG25" s="21"/>
+      <c r="AH25" s="32"/>
+      <c r="AI25" s="32"/>
+      <c r="AJ25" s="48"/>
+      <c r="AK25" s="49" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="26" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>76</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
@@ -9152,28 +9122,21 @@
       <c r="W26" s="10"/>
       <c r="X26" s="10"/>
       <c r="Y26" s="10"/>
-      <c r="AA26" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB26" s="68">
-        <f>AK14</f>
-        <v>-5</v>
-      </c>
-      <c r="AC26" s="71">
-        <f>AK13</f>
-        <v>22.72727272727273</v>
-      </c>
-      <c r="AD26" s="31"/>
+      <c r="AA26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
     </row>
     <row r="27" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B27" s="88">
+      <c r="B27" s="86">
         <v>61</v>
       </c>
       <c r="C27" s="6">
         <f>B27/180*(2.4-0.53)+0.53</f>
         <v>1.1637222222222223</v>
       </c>
-      <c r="D27" s="91">
+      <c r="D27" s="89">
         <f>(C27-1)*180</f>
         <v>29.47000000000002</v>
       </c>
@@ -9198,29 +9161,26 @@
       <c r="W27" s="10"/>
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
-      <c r="AA27" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB27" s="68">
-        <f>AE13</f>
-        <v>-3925.570398689204</v>
-      </c>
-      <c r="AC27" s="72">
-        <f>AE12</f>
-        <v>0.94199104022164515</v>
-      </c>
-      <c r="AD27" s="31"/>
+      <c r="AA27" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB27" s="88">
+        <f>AH22</f>
+        <v>3.3</v>
+      </c>
+      <c r="AC27" s="65"/>
+      <c r="AD27" s="29"/>
     </row>
-    <row r="28" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="76">
+    <row r="28" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="B28" s="74">
         <v>65</v>
       </c>
       <c r="C28" s="6">
-        <f t="shared" ref="C28:C33" si="15">B28/180*(2.4-0.53)+0.53</f>
+        <f t="shared" ref="C28:C33" si="7">B28/180*(2.4-0.53)+0.53</f>
         <v>1.2052777777777779</v>
       </c>
-      <c r="D28" s="91">
-        <f t="shared" ref="D28:D33" si="16">(C28-1)*180</f>
+      <c r="D28" s="89">
+        <f t="shared" ref="D28:D33" si="8">(C28-1)*180</f>
         <v>36.950000000000017</v>
       </c>
       <c r="E28" s="6"/>
@@ -9244,29 +9204,26 @@
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
       <c r="Y28" s="10"/>
-      <c r="AA28" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB28" s="74">
-        <f>AE11</f>
-        <v>4180.4182204512181</v>
-      </c>
-      <c r="AC28" s="75">
-        <f>AE10</f>
-        <v>1.0602056822563426</v>
-      </c>
-      <c r="AD28" s="34"/>
+      <c r="AA28" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB28" s="67">
+        <f>AH21</f>
+        <v>0</v>
+      </c>
+      <c r="AC28" s="46"/>
+      <c r="AD28" s="31"/>
     </row>
     <row r="29" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B29" s="76">
+      <c r="B29" s="74">
         <v>77</v>
       </c>
       <c r="C29" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>1.3299444444444444</v>
       </c>
-      <c r="D29" s="91">
-        <f t="shared" si="16"/>
+      <c r="D29" s="89">
+        <f t="shared" si="8"/>
         <v>59.389999999999986</v>
       </c>
       <c r="E29" s="6"/>
@@ -9290,17 +9247,26 @@
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
       <c r="Y29" s="10"/>
+      <c r="AA29" s="66" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB29" s="67">
+        <f>AE14</f>
+        <v>5</v>
+      </c>
+      <c r="AC29" s="30"/>
+      <c r="AD29" s="31"/>
     </row>
     <row r="30" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B30" s="76">
+      <c r="B30" s="74">
         <v>88</v>
       </c>
       <c r="C30" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>1.4442222222222223</v>
       </c>
-      <c r="D30" s="91">
-        <f t="shared" si="16"/>
+      <c r="D30" s="89">
+        <f t="shared" si="8"/>
         <v>79.960000000000008</v>
       </c>
       <c r="E30" s="6"/>
@@ -9322,45 +9288,159 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
       <c r="Y30" s="3"/>
+      <c r="AA30" s="66" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB30" s="67">
+        <f>AE13</f>
+        <v>0</v>
+      </c>
+      <c r="AC30" s="30"/>
+      <c r="AD30" s="31"/>
     </row>
     <row r="31" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B31" s="76">
+      <c r="B31" s="74">
         <v>95</v>
       </c>
       <c r="C31" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>1.5169444444444444</v>
       </c>
-      <c r="D31" s="91">
-        <f t="shared" si="16"/>
+      <c r="D31" s="89">
+        <f t="shared" si="8"/>
         <v>93.05</v>
       </c>
+      <c r="AA31" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB31" s="91">
+        <f>AB17/100</f>
+        <v>221.53846153846152</v>
+      </c>
+      <c r="AC31" s="30"/>
+      <c r="AD31" s="31"/>
     </row>
     <row r="32" spans="2:41" x14ac:dyDescent="0.3">
-      <c r="B32" s="76">
+      <c r="B32" s="74">
         <v>105</v>
       </c>
       <c r="C32" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>1.6208333333333333</v>
       </c>
-      <c r="D32" s="91">
-        <f t="shared" si="16"/>
+      <c r="D32" s="89">
+        <f t="shared" si="8"/>
         <v>111.75</v>
       </c>
+      <c r="AA32" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB32" s="67">
+        <f>AJ22</f>
+        <v>180</v>
+      </c>
+      <c r="AC32" s="30"/>
+      <c r="AD32" s="31"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="3"/>
     </row>
-    <row r="33" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="83">
+    <row r="33" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="81">
         <v>120</v>
       </c>
       <c r="C33" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="7"/>
         <v>1.7766666666666666</v>
       </c>
-      <c r="D33" s="91">
-        <f t="shared" si="16"/>
+      <c r="D33" s="89">
+        <f t="shared" si="8"/>
         <v>139.79999999999998</v>
       </c>
+      <c r="AA33" s="66" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB33" s="67">
+        <f>AJ21</f>
+        <v>0</v>
+      </c>
+      <c r="AC33" s="30"/>
+      <c r="AD33" s="31"/>
+      <c r="AL33" s="3"/>
+    </row>
+    <row r="34" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="AA34" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB34" s="67">
+        <f>AB22</f>
+        <v>0</v>
+      </c>
+      <c r="AC34" s="68">
+        <f>AB21</f>
+        <v>7447.8773934613901</v>
+      </c>
+      <c r="AD34" s="69">
+        <f>AB20</f>
+        <v>-435.01106108560458</v>
+      </c>
+    </row>
+    <row r="35" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="AA35" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB35" s="67">
+        <f>AB24</f>
+        <v>-23320.445073439671</v>
+      </c>
+      <c r="AC35" s="68">
+        <f>AB23</f>
+        <v>9036.7660560772038</v>
+      </c>
+      <c r="AD35" s="31"/>
+      <c r="AJ35" s="3"/>
+      <c r="AK35" s="3"/>
+    </row>
+    <row r="36" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="AA36" s="66" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB36" s="92">
+        <f>AK24</f>
+        <v>-17.719588605194332</v>
+      </c>
+      <c r="AC36" s="93">
+        <f>AK23</f>
+        <v>26.581693516725558</v>
+      </c>
+      <c r="AD36" s="31"/>
+    </row>
+    <row r="37" spans="2:38" x14ac:dyDescent="0.3">
+      <c r="AA37" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB37" s="67">
+        <f>AE23</f>
+        <v>-3925.570398689204</v>
+      </c>
+      <c r="AC37" s="70">
+        <f>AE22</f>
+        <v>0.94199104022164515</v>
+      </c>
+      <c r="AD37" s="31"/>
+    </row>
+    <row r="38" spans="2:38" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA38" s="71" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB38" s="72">
+        <f>AE21</f>
+        <v>4180.4182204512181</v>
+      </c>
+      <c r="AC38" s="73">
+        <f>AE20</f>
+        <v>1.0602056822563426</v>
+      </c>
+      <c r="AD38" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
compare HiTec to new Turnigy
close enough. model needs work
</commit_message>
<xml_diff>
--- a/myESC-Particle-DEV/saves/calibration20161012.xlsx
+++ b/myESC-Particle-DEV/saves/calibration20161012.xlsx
@@ -665,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -865,6 +865,9 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8748,16 +8751,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>30486</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>83826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9135,9 +9138,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10997,6 +11000,7 @@
         <f>INDEX(LINEST($N$3:$N$9,$O$3:$O$9),1)</f>
         <v>1.0602056822563426</v>
       </c>
+      <c r="AG35" s="102"/>
       <c r="AM35" s="3"/>
       <c r="AN35" s="3"/>
     </row>

</xml_diff>